<commit_message>
updated for parallel processing (working in cluster)
</commit_message>
<xml_diff>
--- a/Utilities/systemConfig.xlsx
+++ b/Utilities/systemConfig.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="27795" windowHeight="14625" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="27795" windowHeight="14625" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="MSE-KKT" sheetId="1" r:id="rId1"/>
@@ -575,7 +575,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.42578125" defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1346,7 +1346,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
@@ -1711,7 +1711,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated working code for group arrival and distributed precoding techniques
</commit_message>
<xml_diff>
--- a/Utilities/systemConfig.xlsx
+++ b/Utilities/systemConfig.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="27795" windowHeight="14625" activeTab="6"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="27795" windowHeight="14625" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="KKT" sheetId="1" r:id="rId1"/>
@@ -13,17 +13,16 @@
     <sheet name="ADMM-WOS" sheetId="3" r:id="rId4"/>
     <sheet name="ADMM-WS" sheetId="4" r:id="rId5"/>
     <sheet name="MSE-O" sheetId="6" r:id="rId6"/>
-    <sheet name="MSE-NM20-0" sheetId="7" r:id="rId7"/>
-    <sheet name="MSE-NM20-20" sheetId="9" r:id="rId8"/>
-    <sheet name="MSE-WM20-0" sheetId="10" r:id="rId9"/>
-    <sheet name="MSE-WM20-20" sheetId="11" r:id="rId10"/>
+    <sheet name="MSE-C" sheetId="7" r:id="rId7"/>
+    <sheet name="MSE-B" sheetId="9" r:id="rId8"/>
+    <sheet name="MSE-L" sheetId="12" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="79">
   <si>
     <t>SkipScheduling</t>
   </si>
@@ -214,36 +213,6 @@
     <t>OL (OTA-10,INT-[20,20])</t>
   </si>
   <si>
-    <t>FOL (OTA-3,INT-[20,0])</t>
-  </si>
-  <si>
-    <t>FOL (OTA-5,INT-[20,0])</t>
-  </si>
-  <si>
-    <t>FOL (OTA-10,INT-[20,0])</t>
-  </si>
-  <si>
-    <t>FOLO (OTA-3,INT-[20,0])</t>
-  </si>
-  <si>
-    <t>FOLOM (OTA-5,INT-[20,0])</t>
-  </si>
-  <si>
-    <t>FOLOM (OTA-3,INT-[20,0])</t>
-  </si>
-  <si>
-    <t>FOLOM (OTA-10,INT-[20,0])</t>
-  </si>
-  <si>
-    <t>FOLM (OTA-5,INT-[20,0])</t>
-  </si>
-  <si>
-    <t>FOLM (OTA-10,INT-[20,0])</t>
-  </si>
-  <si>
-    <t>FOLM (OTA-3,INT-[20,0])</t>
-  </si>
-  <si>
     <t>OLM (OTA-3,INT-[20,20])</t>
   </si>
   <si>
@@ -253,28 +222,43 @@
     <t>OLM (OTA-10,INT-[20,20])</t>
   </si>
   <si>
-    <t>OLOM (OTA-3,INT-[20,20])</t>
-  </si>
-  <si>
-    <t>OLOM (OTA-5,INT-[20,20])</t>
-  </si>
-  <si>
-    <t>OLOM (OTA-10,INT-[20,20])</t>
-  </si>
-  <si>
-    <t>OLO (OTA-3,INT-[20,20])</t>
-  </si>
-  <si>
-    <t>OLO (OTA-5,INT-[20,20])</t>
-  </si>
-  <si>
-    <t>OLO (OTA-10,INT-[20,20])</t>
-  </si>
-  <si>
-    <t>FOLO (OTA-5,INT-[20,0])</t>
-  </si>
-  <si>
-    <t>FOLO (OTA-10,INT-[20,0])</t>
+    <t>E-Optimal</t>
+  </si>
+  <si>
+    <t>OLC (OTA-3,INT-[20,20])</t>
+  </si>
+  <si>
+    <t>OLC (OTA-5,INT-[20,20])</t>
+  </si>
+  <si>
+    <t>OLC (OTA-10,INT-[20,20])</t>
+  </si>
+  <si>
+    <t>OLCM (OTA-3,INT-[20,20])</t>
+  </si>
+  <si>
+    <t>OLCM (OTA-5,INT-[20,20])</t>
+  </si>
+  <si>
+    <t>OLCM (OTA-10,INT-[20,20])</t>
+  </si>
+  <si>
+    <t>OLE (OTA-3,INT-[20,20])</t>
+  </si>
+  <si>
+    <t>OLE (OTA-5,INT-[20,20])</t>
+  </si>
+  <si>
+    <t>OLE (OTA-10,INT-[20,20])</t>
+  </si>
+  <si>
+    <t>OLEM (OTA-3,INT-[20,20])</t>
+  </si>
+  <si>
+    <t>OLEM (OTA-5,INT-[20,20])</t>
+  </si>
+  <si>
+    <t>OLEM (OTA-10,INT-[20,20])</t>
   </si>
 </sst>
 </file>
@@ -1112,369 +1096,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="27.42578125" defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="27.42578125" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="2">
-        <v>3</v>
-      </c>
-      <c r="C7" s="2">
-        <v>5</v>
-      </c>
-      <c r="D7" s="2">
-        <v>10</v>
-      </c>
-      <c r="E7" s="2">
-        <v>3</v>
-      </c>
-      <c r="F7" s="2">
-        <v>5</v>
-      </c>
-      <c r="G7" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="7" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="7">
-        <v>10</v>
-      </c>
-      <c r="C8" s="7">
-        <v>10</v>
-      </c>
-      <c r="D8" s="7">
-        <v>10</v>
-      </c>
-      <c r="E8" s="7">
-        <v>10</v>
-      </c>
-      <c r="F8" s="7">
-        <v>10</v>
-      </c>
-      <c r="G8" s="7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="2">
-        <v>1</v>
-      </c>
-      <c r="C9" s="2">
-        <v>1</v>
-      </c>
-      <c r="D9" s="2">
-        <v>1</v>
-      </c>
-      <c r="E9" s="2">
-        <v>1</v>
-      </c>
-      <c r="F9" s="2">
-        <v>1</v>
-      </c>
-      <c r="G9" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="2">
-        <v>100</v>
-      </c>
-      <c r="C10" s="2">
-        <v>100</v>
-      </c>
-      <c r="D10" s="2">
-        <v>100</v>
-      </c>
-      <c r="E10" s="2">
-        <v>100</v>
-      </c>
-      <c r="F10" s="2">
-        <v>100</v>
-      </c>
-      <c r="G10" s="2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="2">
-        <v>500</v>
-      </c>
-      <c r="C11" s="2">
-        <v>500</v>
-      </c>
-      <c r="D11" s="2">
-        <v>500</v>
-      </c>
-      <c r="E11" s="2">
-        <v>500</v>
-      </c>
-      <c r="F11" s="2">
-        <v>500</v>
-      </c>
-      <c r="G11" s="2">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="2">
-        <v>4</v>
-      </c>
-      <c r="C12" s="2">
-        <v>4</v>
-      </c>
-      <c r="D12" s="2">
-        <v>4</v>
-      </c>
-      <c r="E12" s="2">
-        <v>4</v>
-      </c>
-      <c r="F12" s="2">
-        <v>4</v>
-      </c>
-      <c r="G12" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="2">
-        <v>2</v>
-      </c>
-      <c r="C13" s="2">
-        <v>2</v>
-      </c>
-      <c r="D13" s="2">
-        <v>2</v>
-      </c>
-      <c r="E13" s="2">
-        <v>2</v>
-      </c>
-      <c r="F13" s="2">
-        <v>2</v>
-      </c>
-      <c r="G13" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="2">
-        <v>16</v>
-      </c>
-      <c r="C14" s="2">
-        <v>16</v>
-      </c>
-      <c r="D14" s="2">
-        <v>16</v>
-      </c>
-      <c r="E14" s="2">
-        <v>16</v>
-      </c>
-      <c r="F14" s="2">
-        <v>16</v>
-      </c>
-      <c r="G14" s="2">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="2">
-        <v>2</v>
-      </c>
-      <c r="C15" s="2">
-        <v>2</v>
-      </c>
-      <c r="D15" s="2">
-        <v>2</v>
-      </c>
-      <c r="E15" s="2">
-        <v>2</v>
-      </c>
-      <c r="F15" s="2">
-        <v>2</v>
-      </c>
-      <c r="G15" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="2">
-        <v>4</v>
-      </c>
-      <c r="C16" s="2">
-        <v>4</v>
-      </c>
-      <c r="D16" s="2">
-        <v>4</v>
-      </c>
-      <c r="E16" s="2">
-        <v>4</v>
-      </c>
-      <c r="F16" s="2">
-        <v>4</v>
-      </c>
-      <c r="G16" s="2">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P16"/>
@@ -3159,7 +2780,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.42578125" defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3566,8 +3187,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.42578125" defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3580,22 +3201,22 @@
         <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3672,13 +3293,13 @@
         <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>3</v>
+        <v>57</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>3</v>
+        <v>57</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>3</v>
+        <v>57</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>57</v>
@@ -3727,13 +3348,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="7">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F8" s="7">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G8" s="7">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3741,22 +3362,22 @@
         <v>17</v>
       </c>
       <c r="B9" s="2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C9" s="2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D9" s="2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E9" s="2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F9" s="2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="G9" s="2">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3930,7 +3551,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.42578125" defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3952,13 +3573,13 @@
         <v>62</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4044,13 +3665,13 @@
         <v>3</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>57</v>
+        <v>3</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>57</v>
+        <v>3</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>57</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4090,13 +3711,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="7">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F8" s="7">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G8" s="7">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4104,22 +3725,22 @@
         <v>17</v>
       </c>
       <c r="B9" s="2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C9" s="2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D9" s="2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E9" s="2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F9" s="2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="G9" s="2">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4292,8 +3913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.42578125" defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4306,22 +3927,22 @@
         <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4398,22 +4019,22 @@
         <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>3</v>
+        <v>66</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>3</v>
+        <v>66</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>3</v>
+        <v>66</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4444,13 +4065,13 @@
         <v>16</v>
       </c>
       <c r="B8" s="7">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C8" s="7">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D8" s="7">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E8" s="7">
         <v>10</v>
@@ -4467,22 +4088,22 @@
         <v>17</v>
       </c>
       <c r="B9" s="2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C9" s="2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D9" s="2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E9" s="2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F9" s="2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="G9" s="2">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>